<commit_message>
Cleaned up utils packages.
</commit_message>
<xml_diff>
--- a/AutomationFramework/Resources/Seriti/TestData/Driver.xlsx
+++ b/AutomationFramework/Resources/Seriti/TestData/Driver.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15200" windowHeight="5650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15200" windowHeight="5650"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="157">
   <si>
     <t>Username</t>
   </si>
@@ -76,427 +76,427 @@
     <t>SOUTH AFRICA</t>
   </si>
   <si>
+    <t>TestCaseId</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>Professional</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>strURL</t>
+  </si>
+  <si>
+    <t>https://www.seritisolutions.co.za/demo</t>
+  </si>
+  <si>
+    <t>Johan</t>
+  </si>
+  <si>
+    <t>Johansp02</t>
+  </si>
+  <si>
+    <t>Seriti</t>
+  </si>
+  <si>
+    <t>LoginID</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>TransactionNumber</t>
+  </si>
+  <si>
+    <t>CustomerType</t>
+  </si>
+  <si>
+    <t>TransactionType</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>IdentityNumber</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>CompanyRegNumber</t>
+  </si>
+  <si>
+    <t>CompanyTradingAsName</t>
+  </si>
+  <si>
+    <t>RegistratationDate</t>
+  </si>
+  <si>
+    <t>CompanyYearEnd</t>
+  </si>
+  <si>
+    <t>CompanyVATReg</t>
+  </si>
+  <si>
+    <t>CompanyVATNumber</t>
+  </si>
+  <si>
+    <t>CompanyEntityType</t>
+  </si>
+  <si>
+    <t>CompanyIndustry</t>
+  </si>
+  <si>
+    <t>CompanyIndustrySector</t>
+  </si>
+  <si>
+    <t>CountriesofOperation</t>
+  </si>
+  <si>
+    <t>TurnoverYear</t>
+  </si>
+  <si>
+    <t>Turnover</t>
+  </si>
+  <si>
+    <t>TotalAssetsAmount</t>
+  </si>
+  <si>
+    <t>NumberOfIndTrustees</t>
+  </si>
+  <si>
+    <t>CompanyAddress</t>
+  </si>
+  <si>
+    <t>CompanySuburb</t>
+  </si>
+  <si>
+    <t>CompanyPosition</t>
+  </si>
+  <si>
+    <t>IdentificationType</t>
+  </si>
+  <si>
+    <t>ForeignNational</t>
+  </si>
+  <si>
+    <t>CountryOfBirth</t>
+  </si>
+  <si>
+    <t>ResdidenceCountry</t>
+  </si>
+  <si>
+    <t>EmailAddress</t>
+  </si>
+  <si>
+    <t>MobileNumber</t>
+  </si>
+  <si>
+    <t>AddressLine1</t>
+  </si>
+  <si>
+    <t>Suburb</t>
+  </si>
+  <si>
+    <t>PhysicalAddressDateYears</t>
+  </si>
+  <si>
+    <t>PhysicalAddressDateMonths</t>
+  </si>
+  <si>
+    <t>PostalAddressType</t>
+  </si>
+  <si>
+    <t>PrivateBagNumber</t>
+  </si>
+  <si>
+    <t>ResidentialStatus</t>
+  </si>
+  <si>
+    <t>BondRepayments</t>
+  </si>
+  <si>
+    <t>BondHolder</t>
+  </si>
+  <si>
+    <t>EmpEmploymentType</t>
+  </si>
+  <si>
+    <t>EmpAddress</t>
+  </si>
+  <si>
+    <t>EmpSuburb</t>
+  </si>
+  <si>
+    <t>Occupation</t>
+  </si>
+  <si>
+    <t>OccupationLevel</t>
+  </si>
+  <si>
+    <t>TypeOfIndustry</t>
+  </si>
+  <si>
+    <t>EmployerName</t>
+  </si>
+  <si>
+    <t>CurrentEmploymentYears</t>
+  </si>
+  <si>
+    <t>CurrentEmploymentMonths</t>
+  </si>
+  <si>
+    <t>SalaryDay</t>
+  </si>
+  <si>
+    <t>BasicSalary</t>
+  </si>
+  <si>
+    <t>NettSalary</t>
+  </si>
+  <si>
+    <t>EthnicGroup</t>
+  </si>
+  <si>
+    <t>CorrespondenceLanguage</t>
+  </si>
+  <si>
+    <t>HomeLanguage</t>
+  </si>
+  <si>
+    <t>ContactMethod</t>
+  </si>
+  <si>
+    <t>PreferredStatementMethod</t>
+  </si>
+  <si>
+    <t>RelativeRelationship</t>
+  </si>
+  <si>
+    <t>RelFirstName</t>
+  </si>
+  <si>
+    <t>RelLastName</t>
+  </si>
+  <si>
+    <t>RelTitle</t>
+  </si>
+  <si>
+    <t>RelMobile</t>
+  </si>
+  <si>
+    <t>RelAltMobile</t>
+  </si>
+  <si>
+    <t>RelGender</t>
+  </si>
+  <si>
+    <t>AgreementType</t>
+  </si>
+  <si>
+    <t>PreferredRate</t>
+  </si>
+  <si>
+    <t>InterestRateType</t>
+  </si>
+  <si>
+    <t>FinanceTerm</t>
+  </si>
+  <si>
+    <t>PaymentFrequency</t>
+  </si>
+  <si>
+    <t>PaymentOption</t>
+  </si>
+  <si>
+    <t>AccountType</t>
+  </si>
+  <si>
+    <t>Bank</t>
+  </si>
+  <si>
+    <t>AccountNumber</t>
+  </si>
+  <si>
+    <t>PimaryAccount</t>
+  </si>
+  <si>
+    <t>ActiveYear</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>FirstRegistration</t>
+  </si>
+  <si>
+    <t>VehicleNew</t>
+  </si>
+  <si>
+    <t>OdometerReading</t>
+  </si>
+  <si>
+    <t>RetailPrice</t>
+  </si>
+  <si>
+    <t>CreditCheck</t>
+  </si>
+  <si>
+    <t>ContentOtherCompany</t>
+  </si>
+  <si>
+    <t>CompanyCommunication</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>ApplicationReferenceNumber</t>
+  </si>
+  <si>
+    <t>5aab7e2ff0cd8c75b439518b8ac624252bd183aa851bdefd</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>PRIVATE</t>
+  </si>
+  <si>
+    <t>VEHICLE SALE</t>
+  </si>
+  <si>
+    <t>TESTER</t>
+  </si>
+  <si>
+    <t>AMAZING</t>
+  </si>
+  <si>
+    <t>ABSA TEST ENVIRONMENT</t>
+  </si>
+  <si>
+    <t>ABSA TEST1</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>REG123</t>
+  </si>
+  <si>
+    <t>RSA ID</t>
+  </si>
+  <si>
+    <t>MR</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>first@fakemail.com</t>
+  </si>
+  <si>
+    <t>0789876543</t>
+  </si>
+  <si>
+    <t>Line 1</t>
+  </si>
+  <si>
+    <t>Randburg</t>
+  </si>
+  <si>
+    <t>STREET</t>
+  </si>
+  <si>
+    <t>OWNER BONDED</t>
+  </si>
+  <si>
+    <t>CLIENT</t>
+  </si>
+  <si>
+    <t>EMPLOYED</t>
+  </si>
+  <si>
+    <t>270 Republic Rd</t>
+  </si>
+  <si>
+    <t>ACTOR</t>
+  </si>
+  <si>
+    <t>SKILLED WORKER</t>
+  </si>
+  <si>
+    <t>ARTS AND CULTURE</t>
+  </si>
+  <si>
+    <t>Employer</t>
+  </si>
+  <si>
+    <t>COLOURED</t>
+  </si>
+  <si>
+    <t>ENGLISH</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>SINGLE</t>
+  </si>
+  <si>
+    <t>DISTANT</t>
+  </si>
+  <si>
+    <t>0809874563</t>
+  </si>
+  <si>
+    <t>0809874564</t>
+  </si>
+  <si>
+    <t>MALE</t>
+  </si>
+  <si>
+    <t>INSTALMENT SALE</t>
+  </si>
+  <si>
+    <t>FIXED</t>
+  </si>
+  <si>
+    <t>MONTHLY</t>
+  </si>
+  <si>
+    <t>DEBIT ORDER</t>
+  </si>
+  <si>
+    <t>CHEQUE</t>
+  </si>
+  <si>
+    <t>FIRSTRAND BANK</t>
+  </si>
+  <si>
+    <t>BMW</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>01/01/2017</t>
+  </si>
+  <si>
     <t>Chrome</t>
-  </si>
-  <si>
-    <t>TestCaseId</t>
-  </si>
-  <si>
-    <t>Application</t>
-  </si>
-  <si>
-    <t>Professional</t>
-  </si>
-  <si>
-    <t>ON</t>
-  </si>
-  <si>
-    <t>strURL</t>
-  </si>
-  <si>
-    <t>https://www.seritisolutions.co.za/demo</t>
-  </si>
-  <si>
-    <t>Johan</t>
-  </si>
-  <si>
-    <t>Johansp02</t>
-  </si>
-  <si>
-    <t>Seriti</t>
-  </si>
-  <si>
-    <t>LoginID</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>TransactionNumber</t>
-  </si>
-  <si>
-    <t>CustomerType</t>
-  </si>
-  <si>
-    <t>TransactionType</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
-    <t>Branch</t>
-  </si>
-  <si>
-    <t>IdentityNumber</t>
-  </si>
-  <si>
-    <t>CompanyName</t>
-  </si>
-  <si>
-    <t>CompanyRegNumber</t>
-  </si>
-  <si>
-    <t>CompanyTradingAsName</t>
-  </si>
-  <si>
-    <t>RegistratationDate</t>
-  </si>
-  <si>
-    <t>CompanyYearEnd</t>
-  </si>
-  <si>
-    <t>CompanyVATReg</t>
-  </si>
-  <si>
-    <t>CompanyVATNumber</t>
-  </si>
-  <si>
-    <t>CompanyEntityType</t>
-  </si>
-  <si>
-    <t>CompanyIndustry</t>
-  </si>
-  <si>
-    <t>CompanyIndustrySector</t>
-  </si>
-  <si>
-    <t>CountriesofOperation</t>
-  </si>
-  <si>
-    <t>TurnoverYear</t>
-  </si>
-  <si>
-    <t>Turnover</t>
-  </si>
-  <si>
-    <t>TotalAssetsAmount</t>
-  </si>
-  <si>
-    <t>NumberOfIndTrustees</t>
-  </si>
-  <si>
-    <t>CompanyAddress</t>
-  </si>
-  <si>
-    <t>CompanySuburb</t>
-  </si>
-  <si>
-    <t>CompanyPosition</t>
-  </si>
-  <si>
-    <t>IdentificationType</t>
-  </si>
-  <si>
-    <t>ForeignNational</t>
-  </si>
-  <si>
-    <t>CountryOfBirth</t>
-  </si>
-  <si>
-    <t>ResdidenceCountry</t>
-  </si>
-  <si>
-    <t>EmailAddress</t>
-  </si>
-  <si>
-    <t>MobileNumber</t>
-  </si>
-  <si>
-    <t>AddressLine1</t>
-  </si>
-  <si>
-    <t>Suburb</t>
-  </si>
-  <si>
-    <t>PhysicalAddressDateYears</t>
-  </si>
-  <si>
-    <t>PhysicalAddressDateMonths</t>
-  </si>
-  <si>
-    <t>PostalAddressType</t>
-  </si>
-  <si>
-    <t>PrivateBagNumber</t>
-  </si>
-  <si>
-    <t>ResidentialStatus</t>
-  </si>
-  <si>
-    <t>BondRepayments</t>
-  </si>
-  <si>
-    <t>BondHolder</t>
-  </si>
-  <si>
-    <t>EmpEmploymentType</t>
-  </si>
-  <si>
-    <t>EmpAddress</t>
-  </si>
-  <si>
-    <t>EmpSuburb</t>
-  </si>
-  <si>
-    <t>Occupation</t>
-  </si>
-  <si>
-    <t>OccupationLevel</t>
-  </si>
-  <si>
-    <t>TypeOfIndustry</t>
-  </si>
-  <si>
-    <t>EmployerName</t>
-  </si>
-  <si>
-    <t>CurrentEmploymentYears</t>
-  </si>
-  <si>
-    <t>CurrentEmploymentMonths</t>
-  </si>
-  <si>
-    <t>SalaryDay</t>
-  </si>
-  <si>
-    <t>BasicSalary</t>
-  </si>
-  <si>
-    <t>NettSalary</t>
-  </si>
-  <si>
-    <t>EthnicGroup</t>
-  </si>
-  <si>
-    <t>CorrespondenceLanguage</t>
-  </si>
-  <si>
-    <t>HomeLanguage</t>
-  </si>
-  <si>
-    <t>ContactMethod</t>
-  </si>
-  <si>
-    <t>PreferredStatementMethod</t>
-  </si>
-  <si>
-    <t>RelativeRelationship</t>
-  </si>
-  <si>
-    <t>RelFirstName</t>
-  </si>
-  <si>
-    <t>RelLastName</t>
-  </si>
-  <si>
-    <t>RelTitle</t>
-  </si>
-  <si>
-    <t>RelMobile</t>
-  </si>
-  <si>
-    <t>RelAltMobile</t>
-  </si>
-  <si>
-    <t>RelGender</t>
-  </si>
-  <si>
-    <t>AgreementType</t>
-  </si>
-  <si>
-    <t>PreferredRate</t>
-  </si>
-  <si>
-    <t>InterestRateType</t>
-  </si>
-  <si>
-    <t>FinanceTerm</t>
-  </si>
-  <si>
-    <t>PaymentFrequency</t>
-  </si>
-  <si>
-    <t>PaymentOption</t>
-  </si>
-  <si>
-    <t>AccountType</t>
-  </si>
-  <si>
-    <t>Bank</t>
-  </si>
-  <si>
-    <t>AccountNumber</t>
-  </si>
-  <si>
-    <t>PimaryAccount</t>
-  </si>
-  <si>
-    <t>ActiveYear</t>
-  </si>
-  <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>FirstRegistration</t>
-  </si>
-  <si>
-    <t>VehicleNew</t>
-  </si>
-  <si>
-    <t>OdometerReading</t>
-  </si>
-  <si>
-    <t>RetailPrice</t>
-  </si>
-  <si>
-    <t>CreditCheck</t>
-  </si>
-  <si>
-    <t>ContentOtherCompany</t>
-  </si>
-  <si>
-    <t>CompanyCommunication</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>ApplicationReferenceNumber</t>
-  </si>
-  <si>
-    <t>5aab7e2ff0cd8c75b439518b8ac624252bd183aa851bdefd</t>
-  </si>
-  <si>
-    <t>Create</t>
-  </si>
-  <si>
-    <t>PRIVATE</t>
-  </si>
-  <si>
-    <t>VEHICLE SALE</t>
-  </si>
-  <si>
-    <t>TESTER</t>
-  </si>
-  <si>
-    <t>AMAZING</t>
-  </si>
-  <si>
-    <t>ABSA TEST ENVIRONMENT</t>
-  </si>
-  <si>
-    <t>ABSA TEST1</t>
-  </si>
-  <si>
-    <t>Company Name</t>
-  </si>
-  <si>
-    <t>REG123</t>
-  </si>
-  <si>
-    <t>RSA ID</t>
-  </si>
-  <si>
-    <t>MR</t>
-  </si>
-  <si>
-    <t>False</t>
-  </si>
-  <si>
-    <t>first@fakemail.com</t>
-  </si>
-  <si>
-    <t>0789876543</t>
-  </si>
-  <si>
-    <t>Line 1</t>
-  </si>
-  <si>
-    <t>Randburg</t>
-  </si>
-  <si>
-    <t>STREET</t>
-  </si>
-  <si>
-    <t>OWNER BONDED</t>
-  </si>
-  <si>
-    <t>CLIENT</t>
-  </si>
-  <si>
-    <t>EMPLOYED</t>
-  </si>
-  <si>
-    <t>270 Republic Rd</t>
-  </si>
-  <si>
-    <t>ACTOR</t>
-  </si>
-  <si>
-    <t>SKILLED WORKER</t>
-  </si>
-  <si>
-    <t>ARTS AND CULTURE</t>
-  </si>
-  <si>
-    <t>Employer</t>
-  </si>
-  <si>
-    <t>COLOURED</t>
-  </si>
-  <si>
-    <t>ENGLISH</t>
-  </si>
-  <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
-    <t>SINGLE</t>
-  </si>
-  <si>
-    <t>DISTANT</t>
-  </si>
-  <si>
-    <t>0809874563</t>
-  </si>
-  <si>
-    <t>0809874564</t>
-  </si>
-  <si>
-    <t>MALE</t>
-  </si>
-  <si>
-    <t>INSTALMENT SALE</t>
-  </si>
-  <si>
-    <t>FIXED</t>
-  </si>
-  <si>
-    <t>MONTHLY</t>
-  </si>
-  <si>
-    <t>DEBIT ORDER</t>
-  </si>
-  <si>
-    <t>CHEQUE</t>
-  </si>
-  <si>
-    <t>FIRSTRAND BANK</t>
-  </si>
-  <si>
-    <t>BMW</t>
-  </si>
-  <si>
-    <t>M3</t>
-  </si>
-  <si>
-    <t>01/01/2017</t>
   </si>
 </sst>
 </file>
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -976,22 +976,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>156</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1013,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CZ2"/>
+  <dimension ref="A1:CZ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BU1" workbookViewId="0">
-      <selection activeCell="CB8" sqref="CB8"/>
+    <sheetView topLeftCell="BU1" workbookViewId="0">
+      <selection activeCell="BV9" sqref="BV9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1127,7 +1127,7 @@
   <sheetData>
     <row r="1" spans="1:104" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>8</v>
@@ -1136,283 +1136,283 @@
         <v>9</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>13</v>
       </c>
       <c r="L1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="AG1" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="AH1" s="5" t="s">
         <v>12</v>
       </c>
       <c r="AI1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AL1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AM1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AN1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AO1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AP1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AR1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AS1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="AS1" s="5" t="s">
+      <c r="AT1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="AT1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="AU1" s="5" t="s">
+      <c r="AV1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="AV1" s="5" t="s">
+      <c r="AW1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="AW1" s="5" t="s">
+      <c r="AX1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AY1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="AX1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="AY1" s="5" t="s">
+      <c r="AZ1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="AZ1" s="5" t="s">
+      <c r="BA1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="BA1" s="5" t="s">
+      <c r="BB1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="BB1" s="5" t="s">
+      <c r="BC1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="BC1" s="5" t="s">
+      <c r="BD1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="BD1" s="5" t="s">
+      <c r="BE1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="BE1" s="5" t="s">
+      <c r="BF1" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="BF1" s="5" t="s">
+      <c r="BG1" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="BG1" s="5" t="s">
+      <c r="BH1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="BH1" s="5" t="s">
+      <c r="BI1" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="BI1" s="5" t="s">
+      <c r="BJ1" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="BJ1" s="5" t="s">
+      <c r="BK1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="BK1" s="5" t="s">
+      <c r="BL1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="BL1" s="5" t="s">
+      <c r="BM1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="BM1" s="5" t="s">
+      <c r="BN1" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="BN1" s="5" t="s">
-        <v>84</v>
       </c>
       <c r="BO1" s="5" t="s">
         <v>14</v>
       </c>
       <c r="BP1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="BQ1" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="BQ1" s="5" t="s">
+      <c r="BR1" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="BR1" s="5" t="s">
+      <c r="BS1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="BS1" s="5" t="s">
+      <c r="BT1" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="BT1" s="5" t="s">
+      <c r="BU1" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="BU1" s="5" t="s">
+      <c r="BV1" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="BV1" s="5" t="s">
+      <c r="BW1" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="BW1" s="5" t="s">
+      <c r="BX1" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="BX1" s="5" t="s">
+      <c r="BY1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="BY1" s="5" t="s">
+      <c r="BZ1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="BZ1" s="5" t="s">
+      <c r="CA1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="CA1" s="5" t="s">
+      <c r="CB1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="CB1" s="5" t="s">
+      <c r="CC1" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="CC1" s="5" t="s">
+      <c r="CD1" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="CD1" s="5" t="s">
+      <c r="CE1" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="CE1" s="5" t="s">
+      <c r="CF1" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="CF1" s="5" t="s">
+      <c r="CG1" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="CG1" s="5" t="s">
+      <c r="CH1" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="CH1" s="5" t="s">
+      <c r="CI1" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="CI1" s="5" t="s">
+      <c r="CJ1" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="CJ1" s="5" t="s">
+      <c r="CK1" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="CK1" s="5" t="s">
+      <c r="CL1" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="CL1" s="5" t="s">
+      <c r="CM1" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="CM1" s="5" t="s">
+      <c r="CN1" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="CN1" s="5" t="s">
+      <c r="CO1" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="CO1" s="5" t="s">
+      <c r="CP1" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="CP1" s="5" t="s">
+      <c r="CQ1" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="CQ1" s="5" t="s">
+      <c r="CR1" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="CR1" s="5" t="s">
-        <v>113</v>
       </c>
       <c r="CS1" s="5"/>
       <c r="CT1" s="5"/>
@@ -1425,50 +1425,50 @@
     </row>
     <row r="2" spans="1:104" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="E2" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>114</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="J2" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="K2" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="L2" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="M2" s="10" t="s">
         <v>120</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>121</v>
       </c>
       <c r="N2" s="11">
         <v>8505059408088</v>
       </c>
       <c r="O2" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="P2" s="12" t="s">
         <v>122</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>123</v>
       </c>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -1487,13 +1487,13 @@
       <c r="AE2" s="12"/>
       <c r="AF2" s="12"/>
       <c r="AG2" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="AH2" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="AH2" s="12" t="s">
+      <c r="AI2" s="10" t="s">
         <v>125</v>
-      </c>
-      <c r="AI2" s="10" t="s">
-        <v>126</v>
       </c>
       <c r="AJ2" s="13" t="s">
         <v>15</v>
@@ -1502,16 +1502,16 @@
         <v>15</v>
       </c>
       <c r="AL2" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM2" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="AM2" s="14" t="s">
+      <c r="AN2" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="AN2" s="13" t="s">
+      <c r="AO2" s="13" t="s">
         <v>129</v>
-      </c>
-      <c r="AO2" s="13" t="s">
-        <v>130</v>
       </c>
       <c r="AP2" s="13">
         <v>2</v>
@@ -1520,41 +1520,41 @@
         <v>0</v>
       </c>
       <c r="AR2" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AS2" s="13"/>
       <c r="AT2" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AU2" s="13">
         <v>5000</v>
       </c>
       <c r="AV2" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="AW2" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="AW2" s="13" t="s">
+      <c r="AX2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="AY2" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="AX2" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="AY2" s="13" t="s">
+      <c r="AZ2" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="BA2" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="AZ2" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="BA2" s="13" t="s">
+      <c r="BB2" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="BB2" s="13" t="s">
+      <c r="BC2" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="BC2" s="13" t="s">
+      <c r="BD2" s="13" t="s">
         <v>138</v>
-      </c>
-      <c r="BD2" s="13" t="s">
-        <v>139</v>
       </c>
       <c r="BE2" s="13">
         <v>5</v>
@@ -1572,67 +1572,67 @@
         <v>40000</v>
       </c>
       <c r="BJ2" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="BK2" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="BK2" s="13" t="s">
+      <c r="BL2" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BM2" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="BL2" s="13" t="s">
+      <c r="BN2" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="BM2" s="13" t="s">
+      <c r="BO2" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="BN2" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="BO2" s="13" t="s">
+      <c r="BP2" s="13" t="s">
         <v>143</v>
-      </c>
-      <c r="BP2" s="13" t="s">
-        <v>144</v>
       </c>
       <c r="BQ2" s="13" t="s">
         <v>13</v>
       </c>
       <c r="BR2" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="BS2" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BT2" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="BU2" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="BU2" s="14" t="s">
+      <c r="BV2" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="BV2" s="13" t="s">
+      <c r="BW2" s="13" t="s">
         <v>147</v>
-      </c>
-      <c r="BW2" s="13" t="s">
-        <v>148</v>
       </c>
       <c r="BX2" s="13">
         <v>10</v>
       </c>
       <c r="BY2" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BZ2" s="13">
         <v>60</v>
       </c>
       <c r="CA2" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="CB2" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="CB2" s="13" t="s">
+      <c r="CC2" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="CC2" s="13" t="s">
+      <c r="CD2" s="13" t="s">
         <v>152</v>
-      </c>
-      <c r="CD2" s="13" t="s">
-        <v>153</v>
       </c>
       <c r="CE2" s="13">
         <v>62352049532</v>
@@ -1644,13 +1644,13 @@
         <v>2017</v>
       </c>
       <c r="CH2" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="CI2" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="CI2" s="13" t="s">
+      <c r="CJ2" s="13" t="s">
         <v>155</v>
-      </c>
-      <c r="CJ2" s="13" t="s">
-        <v>156</v>
       </c>
       <c r="CK2" s="13"/>
       <c r="CL2" s="13">
@@ -1660,7 +1660,7 @@
         <v>400000</v>
       </c>
       <c r="CN2" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="CO2" s="13" t="b">
         <v>0</v>
@@ -1672,39 +1672,547 @@
         <v>0</v>
       </c>
       <c r="CR2" s="13">
+        <v>33316092</v>
+      </c>
+    </row>
+    <row r="3" spans="1:104" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="N3" s="11">
+        <v>8505059408088</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="12"/>
+      <c r="Z3" s="12"/>
+      <c r="AA3" s="12"/>
+      <c r="AB3" s="12"/>
+      <c r="AC3" s="12"/>
+      <c r="AD3" s="12"/>
+      <c r="AE3" s="12"/>
+      <c r="AF3" s="12"/>
+      <c r="AG3" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="AH3" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="AI3" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="AJ3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL3" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM3" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN3" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="AO3" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="AP3" s="13">
+        <v>2</v>
+      </c>
+      <c r="AQ3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS3" s="13"/>
+      <c r="AT3" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="AU3" s="13">
+        <v>5000</v>
+      </c>
+      <c r="AV3" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="AW3" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="AX3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="AY3" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="AZ3" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="BA3" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="BB3" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="BC3" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="BD3" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="BE3" s="13">
+        <v>5</v>
+      </c>
+      <c r="BF3" s="13">
+        <v>0</v>
+      </c>
+      <c r="BG3" s="13">
+        <v>20</v>
+      </c>
+      <c r="BH3" s="13">
+        <v>50000</v>
+      </c>
+      <c r="BI3" s="13">
+        <v>40000</v>
+      </c>
+      <c r="BJ3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="BK3" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BL3" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BM3" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="BN3" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="BO3" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="BP3" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="BQ3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="BR3" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="BS3" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="BT3" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="BU3" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV3" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="BW3" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="BX3" s="13">
+        <v>10</v>
+      </c>
+      <c r="BY3" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="BZ3" s="13">
+        <v>60</v>
+      </c>
+      <c r="CA3" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="CB3" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="CC3" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="CD3" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="CE3" s="13">
+        <v>62352049532</v>
+      </c>
+      <c r="CF3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="CG3" s="13">
+        <v>2017</v>
+      </c>
+      <c r="CH3" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="CI3" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="CJ3" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="CK3" s="13"/>
+      <c r="CL3" s="13">
+        <v>100</v>
+      </c>
+      <c r="CM3" s="13">
+        <v>400000</v>
+      </c>
+      <c r="CN3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="CO3" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="CP3" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="CQ3" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="CR3" s="13">
+        <v>33316092</v>
+      </c>
+    </row>
+    <row r="4" spans="1:104" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="N4" s="11">
+        <v>8505059408088</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12"/>
+      <c r="AA4" s="12"/>
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="12"/>
+      <c r="AD4" s="12"/>
+      <c r="AE4" s="12"/>
+      <c r="AF4" s="12"/>
+      <c r="AG4" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="AH4" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="AI4" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="AJ4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL4" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM4" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN4" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="AO4" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="AP4" s="13">
+        <v>2</v>
+      </c>
+      <c r="AQ4" s="13">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS4" s="13"/>
+      <c r="AT4" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="AU4" s="13">
+        <v>5000</v>
+      </c>
+      <c r="AV4" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="AW4" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="AX4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="AY4" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="AZ4" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="BA4" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="BB4" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="BC4" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="BD4" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="BE4" s="13">
+        <v>5</v>
+      </c>
+      <c r="BF4" s="13">
+        <v>0</v>
+      </c>
+      <c r="BG4" s="13">
+        <v>20</v>
+      </c>
+      <c r="BH4" s="13">
+        <v>50000</v>
+      </c>
+      <c r="BI4" s="13">
+        <v>40000</v>
+      </c>
+      <c r="BJ4" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="BK4" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BL4" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BM4" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="BN4" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="BO4" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="BP4" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="BQ4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="BR4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="BS4" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="BT4" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="BU4" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV4" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="BW4" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="BX4" s="13">
+        <v>10</v>
+      </c>
+      <c r="BY4" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="BZ4" s="13">
+        <v>60</v>
+      </c>
+      <c r="CA4" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="CB4" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="CC4" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="CD4" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="CE4" s="13">
+        <v>62352049532</v>
+      </c>
+      <c r="CF4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="CG4" s="13">
+        <v>2017</v>
+      </c>
+      <c r="CH4" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="CI4" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="CJ4" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="CK4" s="13"/>
+      <c r="CL4" s="13">
+        <v>100</v>
+      </c>
+      <c r="CM4" s="13">
+        <v>400000</v>
+      </c>
+      <c r="CN4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="CO4" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="CP4" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="CQ4" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="CR4" s="13">
         <v>33316092</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B4">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BW2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BW2:BW4">
       <formula1>"INSTALMENT SALE,LEASE,RENTAL"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BY2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BY2:BY4">
       <formula1>"FIXED,LINKED"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CK2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CK2:CK4">
       <formula1>"NEW,USED,DEMO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I4">
       <formula1>"VEHICLE SALE, AFTER MARKET, FLEET"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H4">
       <formula1>"PRIVATE,COMPANY"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4">
       <formula1>"Advanced Search,Recently Viewed, Search, Create"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="M2" r:id="rId1" display="test.automation3@test.co.za"/>
     <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="M3" r:id="rId3" display="test.automation3@test.co.za"/>
+    <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="M4" r:id="rId5" display="test.automation3@test.co.za"/>
+    <hyperlink ref="C4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -1723,7 +2231,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>